<commit_message>
plotting scripts, test data, polars and pressure distributions updated
</commit_message>
<xml_diff>
--- a/cp_test.xlsx
+++ b/cp_test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\OneDrive\Documenten\Aerospace Engineering\Python Projects\Wind Tunnel 31\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2c7370cf9d90a8c9/Documenten/Aerospace Engineering/Python Projects/Wind Tunnel 31/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{766998F5-EC8E-4BC3-8C43-ADD3060CFBE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{92900E72-FA43-49EB-84B8-1A5137D37FE4}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="8_{766998F5-EC8E-4BC3-8C43-ADD3060CFBE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4E84A57F-68D7-49D6-8B5D-1090789FDB22}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,6 +33,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -516,9 +519,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2080,15 +2084,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AS50"/>
+  <dimension ref="A1:AQ50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AS5" sqref="A5:AS5"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="AR5" sqref="AR5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2168,7 +2172,7 @@
         <v>883574</v>
       </c>
       <c r="AA1">
-        <v>884059</v>
+        <v>884249</v>
       </c>
       <c r="AB1">
         <v>883448</v>
@@ -2195,37 +2199,31 @@
         <v>881065</v>
       </c>
       <c r="AJ1">
-        <v>880272</v>
+        <v>880038</v>
       </c>
       <c r="AK1">
-        <v>880038</v>
+        <v>881086</v>
       </c>
       <c r="AL1">
-        <v>881086</v>
+        <v>881326</v>
       </c>
       <c r="AM1">
-        <v>881326</v>
+        <v>881502</v>
       </c>
       <c r="AN1">
-        <v>881502</v>
+        <v>882380</v>
       </c>
       <c r="AO1">
-        <v>882380</v>
+        <v>883922</v>
       </c>
       <c r="AP1">
-        <v>883922</v>
+        <v>884003</v>
       </c>
       <c r="AQ1">
-        <v>884003</v>
-      </c>
-      <c r="AR1">
         <v>884132</v>
       </c>
-      <c r="AS1">
-        <v>884249</v>
-      </c>
     </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2292,77 +2290,71 @@
       <c r="V2">
         <v>10.037000000000001</v>
       </c>
-      <c r="W2">
+      <c r="W2" s="2">
         <v>10.538</v>
       </c>
-      <c r="X2">
+      <c r="X2" s="2">
         <v>11.04</v>
       </c>
-      <c r="Y2">
+      <c r="Y2" s="2">
         <v>11.54</v>
       </c>
-      <c r="Z2">
+      <c r="Z2" s="2">
         <v>12.041</v>
       </c>
-      <c r="AA2">
-        <v>12.541</v>
-      </c>
-      <c r="AB2">
+      <c r="AA2" s="2">
+        <v>12.786</v>
+      </c>
+      <c r="AB2" s="2">
         <v>13.045999999999999</v>
       </c>
-      <c r="AC2">
+      <c r="AC2" s="2">
         <v>13.53</v>
       </c>
-      <c r="AD2">
+      <c r="AD2" s="2">
         <v>14.044</v>
       </c>
-      <c r="AE2">
+      <c r="AE2" s="2">
         <v>14.539</v>
       </c>
-      <c r="AF2">
+      <c r="AF2" s="2">
         <v>15.03</v>
       </c>
-      <c r="AG2">
+      <c r="AG2" s="2">
         <v>15.528</v>
       </c>
-      <c r="AH2">
+      <c r="AH2" s="2">
         <v>16.012</v>
       </c>
-      <c r="AI2">
+      <c r="AI2" s="2">
         <v>16.512</v>
       </c>
-      <c r="AJ2">
+      <c r="AJ2" s="2">
         <v>17.007000000000001</v>
       </c>
-      <c r="AK2">
-        <v>17.007000000000001</v>
-      </c>
-      <c r="AL2">
-        <v>16.012</v>
-      </c>
-      <c r="AM2">
+      <c r="AK2" s="2">
+        <v>16.0121</v>
+      </c>
+      <c r="AL2" s="2">
         <v>15.512</v>
       </c>
-      <c r="AN2">
+      <c r="AM2" s="2">
         <v>15.012</v>
       </c>
-      <c r="AO2">
+      <c r="AN2" s="2">
         <v>14.519</v>
       </c>
-      <c r="AP2">
+      <c r="AO2" s="2">
         <v>14.025</v>
       </c>
-      <c r="AQ2">
+      <c r="AP2" s="2">
         <v>13.54</v>
       </c>
-      <c r="AR2">
+      <c r="AQ2" s="2">
         <v>13.041</v>
       </c>
-      <c r="AS2">
-        <v>12.786</v>
-      </c>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>100</v>
       </c>
@@ -2442,7 +2434,7 @@
         <v>-0.13428100000000001</v>
       </c>
       <c r="AA3">
-        <v>-0.186776</v>
+        <v>-0.20932400000000001</v>
       </c>
       <c r="AB3">
         <v>-0.23294200000000001</v>
@@ -2469,37 +2461,31 @@
         <v>-0.62547200000000003</v>
       </c>
       <c r="AJ3">
-        <v>-0.60192400000000001</v>
+        <v>-0.648594</v>
       </c>
       <c r="AK3">
-        <v>-0.648594</v>
+        <v>-0.62358100000000005</v>
       </c>
       <c r="AL3">
-        <v>-0.62358100000000005</v>
+        <v>-0.59192599999999995</v>
       </c>
       <c r="AM3">
-        <v>-0.59192599999999995</v>
+        <v>-0.53808800000000001</v>
       </c>
       <c r="AN3">
-        <v>-0.53808800000000001</v>
+        <v>-0.36381000000000002</v>
       </c>
       <c r="AO3">
-        <v>-0.36381000000000002</v>
+        <v>-0.30522899999999997</v>
       </c>
       <c r="AP3">
-        <v>-0.30522899999999997</v>
+        <v>-0.26976899999999998</v>
       </c>
       <c r="AQ3">
-        <v>-0.26976899999999998</v>
-      </c>
-      <c r="AR3">
         <v>-0.23375000000000001</v>
       </c>
-      <c r="AS3">
-        <v>-0.20932400000000001</v>
-      </c>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>95.199979999999996</v>
       </c>
@@ -2579,7 +2565,7 @@
         <v>-0.14529900000000001</v>
       </c>
       <c r="AA4">
-        <v>-0.19823099999999999</v>
+        <v>-0.221301</v>
       </c>
       <c r="AB4">
         <v>-0.245394</v>
@@ -2606,37 +2592,31 @@
         <v>-0.66435299999999997</v>
       </c>
       <c r="AJ4">
-        <v>-0.62678299999999998</v>
+        <v>-0.68542999999999998</v>
       </c>
       <c r="AK4">
-        <v>-0.68542999999999998</v>
+        <v>-0.65565700000000005</v>
       </c>
       <c r="AL4">
-        <v>-0.65565700000000005</v>
+        <v>-0.62716300000000003</v>
       </c>
       <c r="AM4">
-        <v>-0.62716300000000003</v>
+        <v>-0.58406400000000003</v>
       </c>
       <c r="AN4">
-        <v>-0.58406400000000003</v>
+        <v>-0.43249799999999999</v>
       </c>
       <c r="AO4">
-        <v>-0.43249799999999999</v>
+        <v>-0.35445700000000002</v>
       </c>
       <c r="AP4">
-        <v>-0.35445700000000002</v>
+        <v>-0.286358</v>
       </c>
       <c r="AQ4">
-        <v>-0.286358</v>
-      </c>
-      <c r="AR4">
         <v>-0.24704799999999999</v>
       </c>
-      <c r="AS4">
-        <v>-0.221301</v>
-      </c>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>90.099990000000005</v>
       </c>
@@ -2716,7 +2696,7 @@
         <v>-0.15700700000000001</v>
       </c>
       <c r="AA5">
-        <v>-0.210401</v>
+        <v>-0.23402600000000001</v>
       </c>
       <c r="AB5">
         <v>-0.25862499999999999</v>
@@ -2743,37 +2723,31 @@
         <v>-0.70566399999999996</v>
       </c>
       <c r="AJ5">
-        <v>-0.65319499999999997</v>
+        <v>-0.72456799999999999</v>
       </c>
       <c r="AK5">
-        <v>-0.72456799999999999</v>
+        <v>-0.68973799999999996</v>
       </c>
       <c r="AL5">
-        <v>-0.68973799999999996</v>
+        <v>-0.66460200000000003</v>
       </c>
       <c r="AM5">
-        <v>-0.66460200000000003</v>
+        <v>-0.63291200000000003</v>
       </c>
       <c r="AN5">
-        <v>-0.63291200000000003</v>
+        <v>-0.50547799999999998</v>
       </c>
       <c r="AO5">
-        <v>-0.50547799999999998</v>
+        <v>-0.40676099999999998</v>
       </c>
       <c r="AP5">
-        <v>-0.40676099999999998</v>
+        <v>-0.303983</v>
       </c>
       <c r="AQ5">
-        <v>-0.303983</v>
-      </c>
-      <c r="AR5">
         <v>-0.26117800000000002</v>
       </c>
-      <c r="AS5">
-        <v>-0.23402600000000001</v>
-      </c>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>85.199979999999996</v>
       </c>
@@ -2853,7 +2827,7 @@
         <v>-0.175371</v>
       </c>
       <c r="AA6">
-        <v>-0.22558900000000001</v>
+        <v>-0.24887899999999999</v>
       </c>
       <c r="AB6">
         <v>-0.27033800000000002</v>
@@ -2880,37 +2854,31 @@
         <v>-0.73770100000000005</v>
       </c>
       <c r="AJ6">
-        <v>-0.67147000000000001</v>
+        <v>-0.75107000000000002</v>
       </c>
       <c r="AK6">
-        <v>-0.75107000000000002</v>
+        <v>-0.72204299999999999</v>
       </c>
       <c r="AL6">
-        <v>-0.72204299999999999</v>
+        <v>-0.70049899999999998</v>
       </c>
       <c r="AM6">
-        <v>-0.70049899999999998</v>
+        <v>-0.67512399999999995</v>
       </c>
       <c r="AN6">
-        <v>-0.67512399999999995</v>
+        <v>-0.55101500000000003</v>
       </c>
       <c r="AO6">
-        <v>-0.55101500000000003</v>
+        <v>-0.449152</v>
       </c>
       <c r="AP6">
-        <v>-0.449152</v>
+        <v>-0.31349900000000003</v>
       </c>
       <c r="AQ6">
-        <v>-0.31349900000000003</v>
-      </c>
-      <c r="AR6">
         <v>-0.27421299999999998</v>
       </c>
-      <c r="AS6">
-        <v>-0.24887899999999999</v>
-      </c>
     </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>80.099990000000005</v>
       </c>
@@ -2990,7 +2958,7 @@
         <v>-0.19703300000000001</v>
       </c>
       <c r="AA7">
-        <v>-0.24427399999999999</v>
+        <v>-0.26440900000000001</v>
       </c>
       <c r="AB7">
         <v>-0.28257199999999999</v>
@@ -3017,37 +2985,31 @@
         <v>-0.75520200000000004</v>
       </c>
       <c r="AJ7">
-        <v>-0.67674999999999996</v>
+        <v>-0.76548700000000003</v>
       </c>
       <c r="AK7">
-        <v>-0.76548700000000003</v>
+        <v>-0.74105299999999996</v>
       </c>
       <c r="AL7">
-        <v>-0.74105299999999996</v>
+        <v>-0.72313700000000003</v>
       </c>
       <c r="AM7">
-        <v>-0.72313700000000003</v>
+        <v>-0.704237</v>
       </c>
       <c r="AN7">
-        <v>-0.704237</v>
+        <v>-0.58743699999999999</v>
       </c>
       <c r="AO7">
-        <v>-0.58743699999999999</v>
+        <v>-0.48313499999999998</v>
       </c>
       <c r="AP7">
-        <v>-0.48313499999999998</v>
+        <v>-0.31977800000000001</v>
       </c>
       <c r="AQ7">
-        <v>-0.31977800000000001</v>
-      </c>
-      <c r="AR7">
         <v>-0.285939</v>
       </c>
-      <c r="AS7">
-        <v>-0.26440900000000001</v>
-      </c>
     </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>70.199979999999996</v>
       </c>
@@ -3127,7 +3089,7 @@
         <v>-0.23641599999999999</v>
       </c>
       <c r="AA8">
-        <v>-0.28198099999999998</v>
+        <v>-0.30309399999999997</v>
       </c>
       <c r="AB8">
         <v>-0.3145</v>
@@ -3154,37 +3116,31 @@
         <v>-0.76883299999999999</v>
       </c>
       <c r="AJ8">
-        <v>-0.67640500000000003</v>
+        <v>-0.77547299999999997</v>
       </c>
       <c r="AK8">
-        <v>-0.77547299999999997</v>
+        <v>-0.75598699999999996</v>
       </c>
       <c r="AL8">
-        <v>-0.75598699999999996</v>
+        <v>-0.74518799999999996</v>
       </c>
       <c r="AM8">
-        <v>-0.74518799999999996</v>
+        <v>-0.73880000000000001</v>
       </c>
       <c r="AN8">
-        <v>-0.73880000000000001</v>
+        <v>-0.64860099999999998</v>
       </c>
       <c r="AO8">
-        <v>-0.64860099999999998</v>
+        <v>-0.55103899999999995</v>
       </c>
       <c r="AP8">
-        <v>-0.55103899999999995</v>
+        <v>-0.341862</v>
       </c>
       <c r="AQ8">
-        <v>-0.341862</v>
-      </c>
-      <c r="AR8">
         <v>-0.31758700000000001</v>
       </c>
-      <c r="AS8">
-        <v>-0.30309399999999997</v>
-      </c>
     </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>59.799990000000001</v>
       </c>
@@ -3264,7 +3220,7 @@
         <v>-0.29277300000000001</v>
       </c>
       <c r="AA9">
-        <v>-0.29976799999999998</v>
+        <v>-0.31496200000000002</v>
       </c>
       <c r="AB9">
         <v>-0.31968999999999997</v>
@@ -3291,37 +3247,31 @@
         <v>-0.75725299999999995</v>
       </c>
       <c r="AJ9">
-        <v>-0.66798100000000005</v>
+        <v>-0.76065700000000003</v>
       </c>
       <c r="AK9">
-        <v>-0.76065700000000003</v>
+        <v>-0.74637699999999996</v>
       </c>
       <c r="AL9">
-        <v>-0.74637699999999996</v>
+        <v>-0.73808499999999999</v>
       </c>
       <c r="AM9">
-        <v>-0.73808499999999999</v>
+        <v>-0.74370499999999995</v>
       </c>
       <c r="AN9">
-        <v>-0.74370499999999995</v>
+        <v>-0.696963</v>
       </c>
       <c r="AO9">
-        <v>-0.696963</v>
+        <v>-0.62104199999999998</v>
       </c>
       <c r="AP9">
-        <v>-0.62104199999999998</v>
+        <v>-0.34865600000000002</v>
       </c>
       <c r="AQ9">
-        <v>-0.34865600000000002</v>
-      </c>
-      <c r="AR9">
         <v>-0.32366400000000001</v>
       </c>
-      <c r="AS9">
-        <v>-0.31496200000000002</v>
-      </c>
     </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>55.2</v>
       </c>
@@ -3401,7 +3351,7 @@
         <v>-0.37886199999999998</v>
       </c>
       <c r="AA10">
-        <v>-0.32875900000000002</v>
+        <v>-0.32850699999999999</v>
       </c>
       <c r="AB10">
         <v>-0.324129</v>
@@ -3428,37 +3378,31 @@
         <v>-0.74526300000000001</v>
       </c>
       <c r="AJ10">
-        <v>-0.66167900000000002</v>
+        <v>-0.74822200000000005</v>
       </c>
       <c r="AK10">
-        <v>-0.74822200000000005</v>
+        <v>-0.73672099999999996</v>
       </c>
       <c r="AL10">
-        <v>-0.73672099999999996</v>
+        <v>-0.72885900000000003</v>
       </c>
       <c r="AM10">
-        <v>-0.72885900000000003</v>
+        <v>-0.73795200000000005</v>
       </c>
       <c r="AN10">
-        <v>-0.73795200000000005</v>
+        <v>-0.71622799999999998</v>
       </c>
       <c r="AO10">
-        <v>-0.71622799999999998</v>
+        <v>-0.65893100000000004</v>
       </c>
       <c r="AP10">
-        <v>-0.65893100000000004</v>
+        <v>-0.347528</v>
       </c>
       <c r="AQ10">
-        <v>-0.347528</v>
-      </c>
-      <c r="AR10">
         <v>-0.32756400000000002</v>
       </c>
-      <c r="AS10">
-        <v>-0.32850699999999999</v>
-      </c>
     </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>50.099989999999998</v>
       </c>
@@ -3538,7 +3482,7 @@
         <v>-0.50484499999999999</v>
       </c>
       <c r="AA11">
-        <v>-0.41477199999999997</v>
+        <v>-0.38291700000000001</v>
       </c>
       <c r="AB11">
         <v>-0.35797400000000001</v>
@@ -3565,37 +3509,31 @@
         <v>-0.730491</v>
       </c>
       <c r="AJ11">
-        <v>-0.65460499999999999</v>
+        <v>-0.732352</v>
       </c>
       <c r="AK11">
-        <v>-0.732352</v>
+        <v>-0.72297900000000004</v>
       </c>
       <c r="AL11">
-        <v>-0.72297900000000004</v>
+        <v>-0.71492100000000003</v>
       </c>
       <c r="AM11">
-        <v>-0.71492100000000003</v>
+        <v>-0.72778299999999996</v>
       </c>
       <c r="AN11">
-        <v>-0.72778299999999996</v>
+        <v>-0.73485400000000001</v>
       </c>
       <c r="AO11">
-        <v>-0.73485400000000001</v>
+        <v>-0.69877199999999995</v>
       </c>
       <c r="AP11">
-        <v>-0.69877199999999995</v>
+        <v>-0.356124</v>
       </c>
       <c r="AQ11">
-        <v>-0.356124</v>
-      </c>
-      <c r="AR11">
         <v>-0.35701699999999997</v>
       </c>
-      <c r="AS11">
-        <v>-0.38291700000000001</v>
-      </c>
     </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>45.2</v>
       </c>
@@ -3675,7 +3613,7 @@
         <v>-0.64717999999999998</v>
       </c>
       <c r="AA12">
-        <v>-0.55818500000000004</v>
+        <v>-0.51079200000000002</v>
       </c>
       <c r="AB12">
         <v>-0.46473900000000001</v>
@@ -3702,37 +3640,31 @@
         <v>-0.71585699999999997</v>
       </c>
       <c r="AJ12">
-        <v>-0.65011099999999999</v>
+        <v>-0.71595799999999998</v>
       </c>
       <c r="AK12">
-        <v>-0.71595799999999998</v>
+        <v>-0.70893700000000004</v>
       </c>
       <c r="AL12">
-        <v>-0.70893700000000004</v>
+        <v>-0.70078099999999999</v>
       </c>
       <c r="AM12">
-        <v>-0.70078099999999999</v>
+        <v>-0.71849200000000002</v>
       </c>
       <c r="AN12">
-        <v>-0.71849200000000002</v>
+        <v>-0.757378</v>
       </c>
       <c r="AO12">
-        <v>-0.757378</v>
+        <v>-0.74415799999999999</v>
       </c>
       <c r="AP12">
-        <v>-0.74415799999999999</v>
+        <v>-0.40517799999999998</v>
       </c>
       <c r="AQ12">
-        <v>-0.40517799999999998</v>
-      </c>
-      <c r="AR12">
         <v>-0.458644</v>
       </c>
-      <c r="AS12">
-        <v>-0.51079200000000002</v>
-      </c>
     </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>40.200000000000003</v>
       </c>
@@ -3812,7 +3744,7 @@
         <v>-0.78914099999999998</v>
       </c>
       <c r="AA13">
-        <v>-0.71696000000000004</v>
+        <v>-0.673682</v>
       </c>
       <c r="AB13">
         <v>-0.62695699999999999</v>
@@ -3839,37 +3771,31 @@
         <v>-0.69981199999999999</v>
       </c>
       <c r="AJ13">
-        <v>-0.644312</v>
+        <v>-0.69891099999999995</v>
       </c>
       <c r="AK13">
-        <v>-0.69891099999999995</v>
+        <v>-0.69267400000000001</v>
       </c>
       <c r="AL13">
-        <v>-0.69267400000000001</v>
+        <v>-0.68436699999999995</v>
       </c>
       <c r="AM13">
-        <v>-0.68436699999999995</v>
+        <v>-0.70551600000000003</v>
       </c>
       <c r="AN13">
-        <v>-0.70551600000000003</v>
+        <v>-0.775648</v>
       </c>
       <c r="AO13">
-        <v>-0.775648</v>
+        <v>-0.79239300000000001</v>
       </c>
       <c r="AP13">
-        <v>-0.79239300000000001</v>
+        <v>-0.53173300000000001</v>
       </c>
       <c r="AQ13">
-        <v>-0.53173300000000001</v>
-      </c>
-      <c r="AR13">
         <v>-0.62051999999999996</v>
       </c>
-      <c r="AS13">
-        <v>-0.673682</v>
-      </c>
     </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>35.099989999999998</v>
       </c>
@@ -3949,7 +3875,7 @@
         <v>-0.90375300000000003</v>
       </c>
       <c r="AA14">
-        <v>-0.85241400000000001</v>
+        <v>-0.82098599999999999</v>
       </c>
       <c r="AB14">
         <v>-0.78443799999999997</v>
@@ -3976,37 +3902,31 @@
         <v>-0.68399399999999999</v>
       </c>
       <c r="AJ14">
-        <v>-0.64156899999999994</v>
+        <v>-0.68313900000000005</v>
       </c>
       <c r="AK14">
-        <v>-0.68313900000000005</v>
+        <v>-0.67851600000000001</v>
       </c>
       <c r="AL14">
-        <v>-0.67851600000000001</v>
+        <v>-0.67053200000000002</v>
       </c>
       <c r="AM14">
-        <v>-0.67053200000000002</v>
+        <v>-0.69489199999999995</v>
       </c>
       <c r="AN14">
-        <v>-0.69489199999999995</v>
+        <v>-0.80591400000000002</v>
       </c>
       <c r="AO14">
-        <v>-0.80591400000000002</v>
+        <v>-0.85730300000000004</v>
       </c>
       <c r="AP14">
-        <v>-0.85730300000000004</v>
+        <v>-0.69864400000000004</v>
       </c>
       <c r="AQ14">
-        <v>-0.69864400000000004</v>
-      </c>
-      <c r="AR14">
         <v>-0.77987700000000004</v>
       </c>
-      <c r="AS14">
-        <v>-0.82098599999999999</v>
-      </c>
     </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>30.1</v>
       </c>
@@ -4086,7 +4006,7 @@
         <v>-1.0048250000000001</v>
       </c>
       <c r="AA15">
-        <v>-0.96984300000000001</v>
+        <v>-0.94775699999999996</v>
       </c>
       <c r="AB15">
         <v>-0.92133500000000002</v>
@@ -4113,37 +4033,31 @@
         <v>-0.666018</v>
       </c>
       <c r="AJ15">
-        <v>-0.63776900000000003</v>
+        <v>-0.66595800000000005</v>
       </c>
       <c r="AK15">
-        <v>-0.66595800000000005</v>
+        <v>-0.66203599999999996</v>
       </c>
       <c r="AL15">
-        <v>-0.66203599999999996</v>
+        <v>-0.65538399999999997</v>
       </c>
       <c r="AM15">
-        <v>-0.65538399999999997</v>
+        <v>-0.68299399999999999</v>
       </c>
       <c r="AN15">
-        <v>-0.68299399999999999</v>
+        <v>-0.84076799999999996</v>
       </c>
       <c r="AO15">
-        <v>-0.84076799999999996</v>
+        <v>-0.93426399999999998</v>
       </c>
       <c r="AP15">
-        <v>-0.93426399999999998</v>
+        <v>-0.85407900000000003</v>
       </c>
       <c r="AQ15">
-        <v>-0.85407900000000003</v>
-      </c>
-      <c r="AR15">
         <v>-0.91737000000000002</v>
       </c>
-      <c r="AS15">
-        <v>-0.94775699999999996</v>
-      </c>
     </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>25</v>
       </c>
@@ -4223,7 +4137,7 @@
         <v>-1.112725</v>
       </c>
       <c r="AA16">
-        <v>-1.0910299999999999</v>
+        <v>-1.0765819999999999</v>
       </c>
       <c r="AB16">
         <v>-1.058093</v>
@@ -4250,37 +4164,31 @@
         <v>-0.64900999999999998</v>
       </c>
       <c r="AJ16">
-        <v>-0.62922500000000003</v>
+        <v>-0.64970499999999998</v>
       </c>
       <c r="AK16">
-        <v>-0.64970499999999998</v>
+        <v>-0.64579600000000004</v>
       </c>
       <c r="AL16">
-        <v>-0.64579600000000004</v>
+        <v>-0.63891399999999998</v>
       </c>
       <c r="AM16">
-        <v>-0.63891399999999998</v>
+        <v>-0.66782200000000003</v>
       </c>
       <c r="AN16">
-        <v>-0.66782200000000003</v>
+        <v>-0.86507500000000004</v>
       </c>
       <c r="AO16">
-        <v>-0.86507500000000004</v>
+        <v>-1.0007010000000001</v>
       </c>
       <c r="AP16">
-        <v>-1.0007010000000001</v>
+        <v>-1.008006</v>
       </c>
       <c r="AQ16">
-        <v>-1.008006</v>
-      </c>
-      <c r="AR16">
         <v>-1.055231</v>
       </c>
-      <c r="AS16">
-        <v>-1.0765819999999999</v>
-      </c>
     </row>
-    <row r="17" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>20</v>
       </c>
@@ -4360,7 +4268,7 @@
         <v>-1.2558670000000001</v>
       </c>
       <c r="AA17">
-        <v>-1.2459789999999999</v>
+        <v>-1.238475</v>
       </c>
       <c r="AB17">
         <v>-1.225962</v>
@@ -4387,37 +4295,31 @@
         <v>-0.63556299999999999</v>
       </c>
       <c r="AJ17">
-        <v>-0.624363</v>
+        <v>-0.63671299999999997</v>
       </c>
       <c r="AK17">
-        <v>-0.63671299999999997</v>
+        <v>-0.63284600000000002</v>
       </c>
       <c r="AL17">
-        <v>-0.63284600000000002</v>
+        <v>-0.62697499999999995</v>
       </c>
       <c r="AM17">
-        <v>-0.62697499999999995</v>
+        <v>-0.65677600000000003</v>
       </c>
       <c r="AN17">
-        <v>-0.65677600000000003</v>
+        <v>-0.90570099999999998</v>
       </c>
       <c r="AO17">
-        <v>-0.90570099999999998</v>
+        <v>-1.087545</v>
       </c>
       <c r="AP17">
-        <v>-1.087545</v>
+        <v>-1.1907970000000001</v>
       </c>
       <c r="AQ17">
-        <v>-1.1907970000000001</v>
-      </c>
-      <c r="AR17">
         <v>-1.224099</v>
       </c>
-      <c r="AS17">
-        <v>-1.238475</v>
-      </c>
     </row>
-    <row r="18" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>15.1</v>
       </c>
@@ -4497,7 +4399,7 @@
         <v>-1.437071</v>
       </c>
       <c r="AA18">
-        <v>-1.43973</v>
+        <v>-1.438131</v>
       </c>
       <c r="AB18">
         <v>-1.4332229999999999</v>
@@ -4524,37 +4426,31 @@
         <v>-0.62363199999999996</v>
       </c>
       <c r="AJ18">
-        <v>-0.61929500000000004</v>
+        <v>-0.62575899999999995</v>
       </c>
       <c r="AK18">
-        <v>-0.62575899999999995</v>
+        <v>-0.62124500000000005</v>
       </c>
       <c r="AL18">
-        <v>-0.62124500000000005</v>
+        <v>-0.61532299999999995</v>
       </c>
       <c r="AM18">
-        <v>-0.61532299999999995</v>
+        <v>-0.64319599999999999</v>
       </c>
       <c r="AN18">
-        <v>-0.64319599999999999</v>
+        <v>-0.93546799999999997</v>
       </c>
       <c r="AO18">
-        <v>-0.93546799999999997</v>
+        <v>-1.163781</v>
       </c>
       <c r="AP18">
-        <v>-1.163781</v>
+        <v>-1.411492</v>
       </c>
       <c r="AQ18">
-        <v>-1.411492</v>
-      </c>
-      <c r="AR18">
         <v>-1.4313100000000001</v>
       </c>
-      <c r="AS18">
-        <v>-1.438131</v>
-      </c>
     </row>
-    <row r="19" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>10.1</v>
       </c>
@@ -4634,7 +4530,7 @@
         <v>-1.7213970000000001</v>
       </c>
       <c r="AA19">
-        <v>-1.7390140000000001</v>
+        <v>-1.7451810000000001</v>
       </c>
       <c r="AB19">
         <v>-1.747652</v>
@@ -4661,37 +4557,31 @@
         <v>-0.61806700000000003</v>
       </c>
       <c r="AJ19">
-        <v>-0.61845300000000003</v>
+        <v>-0.62129199999999996</v>
       </c>
       <c r="AK19">
-        <v>-0.62129199999999996</v>
+        <v>-0.61524699999999999</v>
       </c>
       <c r="AL19">
-        <v>-0.61524699999999999</v>
+        <v>-0.60940799999999995</v>
       </c>
       <c r="AM19">
-        <v>-0.60940799999999995</v>
+        <v>-0.63352799999999998</v>
       </c>
       <c r="AN19">
-        <v>-0.63352799999999998</v>
+        <v>-0.95811100000000005</v>
       </c>
       <c r="AO19">
-        <v>-0.95811100000000005</v>
+        <v>-1.2318020000000001</v>
       </c>
       <c r="AP19">
-        <v>-1.2318020000000001</v>
+        <v>-1.741222</v>
       </c>
       <c r="AQ19">
-        <v>-1.741222</v>
-      </c>
-      <c r="AR19">
         <v>-1.745568</v>
       </c>
-      <c r="AS19">
-        <v>-1.7451810000000001</v>
-      </c>
     </row>
-    <row r="20" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>8.9</v>
       </c>
@@ -4771,7 +4661,7 @@
         <v>-1.8468260000000001</v>
       </c>
       <c r="AA20">
-        <v>-1.870744</v>
+        <v>-1.8797550000000001</v>
       </c>
       <c r="AB20">
         <v>-1.885229</v>
@@ -4798,37 +4688,31 @@
         <v>-0.61821199999999998</v>
       </c>
       <c r="AJ20">
-        <v>-0.61983999999999995</v>
+        <v>-0.62212299999999998</v>
       </c>
       <c r="AK20">
-        <v>-0.62212299999999998</v>
+        <v>-0.61485500000000004</v>
       </c>
       <c r="AL20">
-        <v>-0.61485500000000004</v>
+        <v>-0.60935899999999998</v>
       </c>
       <c r="AM20">
-        <v>-0.60935899999999998</v>
+        <v>-0.63198100000000001</v>
       </c>
       <c r="AN20">
-        <v>-0.63198100000000001</v>
+        <v>-0.95893600000000001</v>
       </c>
       <c r="AO20">
-        <v>-0.95893600000000001</v>
+        <v>-1.239724</v>
       </c>
       <c r="AP20">
-        <v>-1.239724</v>
+        <v>-1.8841840000000001</v>
       </c>
       <c r="AQ20">
-        <v>-1.8841840000000001</v>
-      </c>
-      <c r="AR20">
         <v>-1.883483</v>
       </c>
-      <c r="AS20">
-        <v>-1.8797550000000001</v>
-      </c>
     </row>
-    <row r="21" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>7.1</v>
       </c>
@@ -4908,7 +4792,7 @@
         <v>-1.9989479999999999</v>
       </c>
       <c r="AA21">
-        <v>-2.030195</v>
+        <v>-2.0432730000000001</v>
       </c>
       <c r="AB21">
         <v>-2.0534409999999998</v>
@@ -4935,37 +4819,31 @@
         <v>-0.62190900000000005</v>
       </c>
       <c r="AJ21">
-        <v>-0.623363</v>
+        <v>-0.62659200000000004</v>
       </c>
       <c r="AK21">
-        <v>-0.62659200000000004</v>
+        <v>-0.61869200000000002</v>
       </c>
       <c r="AL21">
-        <v>-0.61869200000000002</v>
+        <v>-0.61294599999999999</v>
       </c>
       <c r="AM21">
-        <v>-0.61294599999999999</v>
+        <v>-0.63474699999999995</v>
       </c>
       <c r="AN21">
-        <v>-0.63474699999999995</v>
+        <v>-0.96409100000000003</v>
       </c>
       <c r="AO21">
-        <v>-0.96409100000000003</v>
+        <v>-1.2532080000000001</v>
       </c>
       <c r="AP21">
-        <v>-1.2532080000000001</v>
+        <v>-2.0592899999999998</v>
       </c>
       <c r="AQ21">
-        <v>-2.0592899999999998</v>
-      </c>
-      <c r="AR21">
         <v>-2.0505939999999998</v>
       </c>
-      <c r="AS21">
-        <v>-2.0432730000000001</v>
-      </c>
     </row>
-    <row r="22" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>5.5</v>
       </c>
@@ -5045,7 +4923,7 @@
         <v>-2.2006079999999999</v>
       </c>
       <c r="AA22">
-        <v>-2.2447780000000002</v>
+        <v>-2.2624590000000002</v>
       </c>
       <c r="AB22">
         <v>-2.2777820000000002</v>
@@ -5072,37 +4950,31 @@
         <v>-1.718642</v>
       </c>
       <c r="AJ22">
-        <v>-1.0412840000000001</v>
+        <v>-1.8235079999999999</v>
       </c>
       <c r="AK22">
-        <v>-1.8235079999999999</v>
+        <v>-1.609332</v>
       </c>
       <c r="AL22">
-        <v>-1.609332</v>
+        <v>-1.4879009999999999</v>
       </c>
       <c r="AM22">
-        <v>-1.4879009999999999</v>
+        <v>-1.477778</v>
       </c>
       <c r="AN22">
-        <v>-1.477778</v>
+        <v>-0.95084100000000005</v>
       </c>
       <c r="AO22">
-        <v>-0.95084100000000005</v>
+        <v>-1.173732</v>
       </c>
       <c r="AP22">
-        <v>-1.173732</v>
+        <v>-2.287747</v>
       </c>
       <c r="AQ22">
-        <v>-2.287747</v>
-      </c>
-      <c r="AR22">
         <v>-2.2742460000000002</v>
       </c>
-      <c r="AS22">
-        <v>-2.2624590000000002</v>
-      </c>
     </row>
-    <row r="23" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>4.3</v>
       </c>
@@ -5182,7 +5054,7 @@
         <v>-2.5020910000000001</v>
       </c>
       <c r="AA23">
-        <v>-2.5531679999999999</v>
+        <v>-2.5773000000000001</v>
       </c>
       <c r="AB23">
         <v>-2.5980129999999999</v>
@@ -5209,37 +5081,31 @@
         <v>-0.65106600000000003</v>
       </c>
       <c r="AJ23">
-        <v>-0.63732900000000003</v>
+        <v>-0.65717499999999995</v>
       </c>
       <c r="AK23">
-        <v>-0.65717499999999995</v>
+        <v>-0.64595000000000002</v>
       </c>
       <c r="AL23">
-        <v>-0.64595000000000002</v>
+        <v>-0.64019599999999999</v>
       </c>
       <c r="AM23">
-        <v>-0.64019599999999999</v>
+        <v>-0.65937500000000004</v>
       </c>
       <c r="AN23">
-        <v>-0.65937500000000004</v>
+        <v>-0.95954899999999999</v>
       </c>
       <c r="AO23">
-        <v>-0.95954899999999999</v>
+        <v>-1.2520169999999999</v>
       </c>
       <c r="AP23">
-        <v>-1.2520169999999999</v>
+        <v>-2.6221619999999999</v>
       </c>
       <c r="AQ23">
-        <v>-2.6221619999999999</v>
-      </c>
-      <c r="AR23">
         <v>-2.5955270000000001</v>
       </c>
-      <c r="AS23">
-        <v>-2.5773000000000001</v>
-      </c>
     </row>
-    <row r="24" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>3.1</v>
       </c>
@@ -5319,7 +5185,7 @@
         <v>-2.9661179999999998</v>
       </c>
       <c r="AA24">
-        <v>-3.030856</v>
+        <v>-3.0599660000000002</v>
       </c>
       <c r="AB24">
         <v>-3.0849310000000001</v>
@@ -5346,37 +5212,31 @@
         <v>-0.72284800000000005</v>
       </c>
       <c r="AJ24">
-        <v>-0.656698</v>
+        <v>-0.72887000000000002</v>
       </c>
       <c r="AK24">
-        <v>-0.72887000000000002</v>
+        <v>-0.71563200000000005</v>
       </c>
       <c r="AL24">
-        <v>-0.71563200000000005</v>
+        <v>-0.70918099999999995</v>
       </c>
       <c r="AM24">
-        <v>-0.70918099999999995</v>
+        <v>-0.72681600000000002</v>
       </c>
       <c r="AN24">
-        <v>-0.72681600000000002</v>
+        <v>-0.95885100000000001</v>
       </c>
       <c r="AO24">
-        <v>-0.95885100000000001</v>
+        <v>-1.2471429999999999</v>
       </c>
       <c r="AP24">
-        <v>-1.2471429999999999</v>
+        <v>-3.1130810000000002</v>
       </c>
       <c r="AQ24">
-        <v>-3.1130810000000002</v>
-      </c>
-      <c r="AR24">
         <v>-3.0817199999999998</v>
       </c>
-      <c r="AS24">
-        <v>-3.0599660000000002</v>
-      </c>
     </row>
-    <row r="25" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>1.8</v>
       </c>
@@ -5456,7 +5316,7 @@
         <v>-4.0702720000000001</v>
       </c>
       <c r="AA25">
-        <v>-4.1927989999999999</v>
+        <v>-4.2810509999999997</v>
       </c>
       <c r="AB25">
         <v>-4.3391000000000002</v>
@@ -5483,37 +5343,31 @@
         <v>-0.98666699999999996</v>
       </c>
       <c r="AJ25">
-        <v>-0.71675900000000003</v>
+        <v>-0.993394</v>
       </c>
       <c r="AK25">
-        <v>-0.993394</v>
+        <v>-0.97692100000000004</v>
       </c>
       <c r="AL25">
-        <v>-0.97692100000000004</v>
+        <v>-0.95995200000000003</v>
       </c>
       <c r="AM25">
-        <v>-0.95995200000000003</v>
+        <v>-0.96884800000000004</v>
       </c>
       <c r="AN25">
-        <v>-0.96884800000000004</v>
+        <v>-0.95250999999999997</v>
       </c>
       <c r="AO25">
-        <v>-0.95250999999999997</v>
+        <v>-1.2422089999999999</v>
       </c>
       <c r="AP25">
-        <v>-1.2422089999999999</v>
+        <v>-4.5000390000000001</v>
       </c>
       <c r="AQ25">
-        <v>-4.5000390000000001</v>
-      </c>
-      <c r="AR25">
         <v>-4.3373980000000003</v>
       </c>
-      <c r="AS25">
-        <v>-4.2810509999999997</v>
-      </c>
     </row>
-    <row r="26" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>0.8</v>
       </c>
@@ -5593,7 +5447,7 @@
         <v>-4.9783340000000003</v>
       </c>
       <c r="AA26">
-        <v>-5.1296390000000001</v>
+        <v>-5.2053760000000002</v>
       </c>
       <c r="AB26">
         <v>-5.2764280000000001</v>
@@ -5620,37 +5474,31 @@
         <v>-1.022413</v>
       </c>
       <c r="AJ26">
-        <v>-0.72220899999999999</v>
+        <v>-1.0332460000000001</v>
       </c>
       <c r="AK26">
-        <v>-1.0332460000000001</v>
+        <v>-1.002583</v>
       </c>
       <c r="AL26">
-        <v>-1.002583</v>
+        <v>-0.98973599999999995</v>
       </c>
       <c r="AM26">
-        <v>-0.98973599999999995</v>
+        <v>-1.0092019999999999</v>
       </c>
       <c r="AN26">
-        <v>-1.0092019999999999</v>
+        <v>-0.95642000000000005</v>
       </c>
       <c r="AO26">
-        <v>-0.95642000000000005</v>
+        <v>-1.2457879999999999</v>
       </c>
       <c r="AP26">
-        <v>-1.2457879999999999</v>
+        <v>-5.3837549999999998</v>
       </c>
       <c r="AQ26">
-        <v>-5.3837549999999998</v>
-      </c>
-      <c r="AR26">
         <v>-5.2719170000000002</v>
       </c>
-      <c r="AS26">
-        <v>-5.2053760000000002</v>
-      </c>
     </row>
-    <row r="27" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>0</v>
       </c>
@@ -5730,7 +5578,7 @@
         <v>-2.9533849999999999</v>
       </c>
       <c r="AA27">
-        <v>-3.1756419999999999</v>
+        <v>-3.2816749999999999</v>
       </c>
       <c r="AB27">
         <v>-3.3846500000000002</v>
@@ -5757,37 +5605,31 @@
         <v>-0.53077799999999997</v>
       </c>
       <c r="AJ27">
-        <v>-0.27369100000000002</v>
+        <v>-0.56043200000000004</v>
       </c>
       <c r="AK27">
-        <v>-0.56043200000000004</v>
+        <v>-0.50212400000000001</v>
       </c>
       <c r="AL27">
-        <v>-0.50212400000000001</v>
+        <v>-0.45935799999999999</v>
       </c>
       <c r="AM27">
-        <v>-0.45935799999999999</v>
+        <v>-0.44897700000000001</v>
       </c>
       <c r="AN27">
-        <v>-0.44897700000000001</v>
+        <v>-0.58567199999999997</v>
       </c>
       <c r="AO27">
-        <v>-0.58567199999999997</v>
+        <v>-0.86295200000000005</v>
       </c>
       <c r="AP27">
-        <v>-0.86295200000000005</v>
+        <v>-3.5540660000000002</v>
       </c>
       <c r="AQ27">
-        <v>-3.5540660000000002</v>
-      </c>
-      <c r="AR27">
         <v>-3.3783159999999999</v>
       </c>
-      <c r="AS27">
-        <v>-3.2816749999999999</v>
-      </c>
     </row>
-    <row r="28" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>0</v>
       </c>
@@ -5867,7 +5709,7 @@
         <v>-2.966126</v>
       </c>
       <c r="AA28">
-        <v>-3.1893210000000001</v>
+        <v>-3.2959640000000001</v>
       </c>
       <c r="AB28">
         <v>-3.3987859999999999</v>
@@ -5894,37 +5736,31 @@
         <v>-0.53314499999999998</v>
       </c>
       <c r="AJ28">
-        <v>-0.27473199999999998</v>
+        <v>-0.56268099999999999</v>
       </c>
       <c r="AK28">
-        <v>-0.56268099999999999</v>
+        <v>-0.50439199999999995</v>
       </c>
       <c r="AL28">
-        <v>-0.50439199999999995</v>
+        <v>-0.461372</v>
       </c>
       <c r="AM28">
-        <v>-0.461372</v>
+        <v>-0.450876</v>
       </c>
       <c r="AN28">
-        <v>-0.450876</v>
+        <v>-0.58822600000000003</v>
       </c>
       <c r="AO28">
-        <v>-0.58822600000000003</v>
+        <v>-0.86670899999999995</v>
       </c>
       <c r="AP28">
-        <v>-0.86670899999999995</v>
+        <v>-3.5694669999999999</v>
       </c>
       <c r="AQ28">
-        <v>-3.5694669999999999</v>
-      </c>
-      <c r="AR28">
         <v>-3.3927339999999999</v>
       </c>
-      <c r="AS28">
-        <v>-3.2959640000000001</v>
-      </c>
     </row>
-    <row r="29" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>0.6</v>
       </c>
@@ -6004,7 +5840,7 @@
         <v>0.64154599999999995</v>
       </c>
       <c r="AA29">
-        <v>0.59190699999999996</v>
+        <v>0.56737400000000004</v>
       </c>
       <c r="AB29">
         <v>0.54310999999999998</v>
@@ -6031,37 +5867,31 @@
         <v>0.92859899999999995</v>
       </c>
       <c r="AJ29">
-        <v>0.96028100000000005</v>
+        <v>0.92205000000000004</v>
       </c>
       <c r="AK29">
-        <v>0.92205000000000004</v>
+        <v>0.93240699999999999</v>
       </c>
       <c r="AL29">
-        <v>0.93240699999999999</v>
+        <v>0.941608</v>
       </c>
       <c r="AM29">
-        <v>0.941608</v>
+        <v>0.94548299999999996</v>
       </c>
       <c r="AN29">
-        <v>0.94548299999999996</v>
+        <v>0.91396599999999995</v>
       </c>
       <c r="AO29">
-        <v>0.91396599999999995</v>
+        <v>0.87428799999999995</v>
       </c>
       <c r="AP29">
-        <v>0.87428799999999995</v>
+        <v>0.50032799999999999</v>
       </c>
       <c r="AQ29">
-        <v>0.50032799999999999</v>
-      </c>
-      <c r="AR29">
         <v>0.54442000000000002</v>
       </c>
-      <c r="AS29">
-        <v>0.56737400000000004</v>
-      </c>
     </row>
-    <row r="30" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>1.6</v>
       </c>
@@ -6141,7 +5971,7 @@
         <v>0.97039399999999998</v>
       </c>
       <c r="AA30">
-        <v>0.95955599999999996</v>
+        <v>0.95372100000000004</v>
       </c>
       <c r="AB30">
         <v>0.94767400000000002</v>
@@ -6168,37 +5998,31 @@
         <v>0.98997400000000002</v>
       </c>
       <c r="AJ30">
-        <v>0.98151200000000005</v>
+        <v>0.990985</v>
       </c>
       <c r="AK30">
-        <v>0.990985</v>
+        <v>0.98783299999999996</v>
       </c>
       <c r="AL30">
-        <v>0.98783299999999996</v>
+        <v>0.98631400000000002</v>
       </c>
       <c r="AM30">
-        <v>0.98631400000000002</v>
+        <v>0.98489599999999999</v>
       </c>
       <c r="AN30">
-        <v>0.98489599999999999</v>
+        <v>0.98631100000000005</v>
       </c>
       <c r="AO30">
-        <v>0.98631100000000005</v>
+        <v>0.98658199999999996</v>
       </c>
       <c r="AP30">
-        <v>0.98658199999999996</v>
+        <v>0.93620000000000003</v>
       </c>
       <c r="AQ30">
-        <v>0.93620000000000003</v>
-      </c>
-      <c r="AR30">
         <v>0.94796899999999995</v>
       </c>
-      <c r="AS30">
-        <v>0.95372100000000004</v>
-      </c>
     </row>
-    <row r="31" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>3</v>
       </c>
@@ -6278,7 +6102,7 @@
         <v>0.96437300000000004</v>
       </c>
       <c r="AA31">
-        <v>0.97019699999999998</v>
+        <v>0.97268900000000003</v>
       </c>
       <c r="AB31">
         <v>0.97444900000000001</v>
@@ -6305,37 +6129,31 @@
         <v>0.90107899999999996</v>
       </c>
       <c r="AJ31">
-        <v>0.87833000000000006</v>
+        <v>0.90639000000000003</v>
       </c>
       <c r="AK31">
-        <v>0.90639000000000003</v>
+        <v>0.89608299999999996</v>
       </c>
       <c r="AL31">
-        <v>0.89608299999999996</v>
+        <v>0.88876299999999997</v>
       </c>
       <c r="AM31">
-        <v>0.88876299999999997</v>
+        <v>0.88375199999999998</v>
       </c>
       <c r="AN31">
-        <v>0.88375199999999998</v>
+        <v>0.90222400000000003</v>
       </c>
       <c r="AO31">
-        <v>0.90222400000000003</v>
+        <v>0.91908800000000002</v>
       </c>
       <c r="AP31">
-        <v>0.91908800000000002</v>
+        <v>0.97701499999999997</v>
       </c>
       <c r="AQ31">
-        <v>0.97701499999999997</v>
-      </c>
-      <c r="AR31">
         <v>0.97444699999999995</v>
       </c>
-      <c r="AS31">
-        <v>0.97268900000000003</v>
-      </c>
     </row>
-    <row r="32" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>4.2</v>
       </c>
@@ -6415,7 +6233,7 @@
         <v>0.91006600000000004</v>
       </c>
       <c r="AA32">
-        <v>0.92356700000000003</v>
+        <v>0.92957000000000001</v>
       </c>
       <c r="AB32">
         <v>0.93507200000000001</v>
@@ -6442,37 +6260,31 @@
         <v>0.82277299999999998</v>
       </c>
       <c r="AJ32">
-        <v>0.79031700000000005</v>
+        <v>0.82998499999999997</v>
       </c>
       <c r="AK32">
-        <v>0.82998499999999997</v>
+        <v>0.81689100000000003</v>
       </c>
       <c r="AL32">
-        <v>0.81689100000000003</v>
+        <v>0.80706100000000003</v>
       </c>
       <c r="AM32">
-        <v>0.80706100000000003</v>
+        <v>0.80046300000000004</v>
       </c>
       <c r="AN32">
-        <v>0.80046300000000004</v>
+        <v>0.82707200000000003</v>
       </c>
       <c r="AO32">
-        <v>0.82707200000000003</v>
+        <v>0.84997100000000003</v>
       </c>
       <c r="AP32">
-        <v>0.84997100000000003</v>
+        <v>0.94424300000000005</v>
       </c>
       <c r="AQ32">
-        <v>0.94424300000000005</v>
-      </c>
-      <c r="AR32">
         <v>0.93487100000000001</v>
       </c>
-      <c r="AS32">
-        <v>0.92957000000000001</v>
-      </c>
     </row>
-    <row r="33" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>5.4</v>
       </c>
@@ -6552,7 +6364,7 @@
         <v>0.83743800000000002</v>
       </c>
       <c r="AA33">
-        <v>0.85423700000000002</v>
+        <v>0.86193200000000003</v>
       </c>
       <c r="AB33">
         <v>0.86904800000000004</v>
@@ -6579,37 +6391,31 @@
         <v>0.74616400000000005</v>
       </c>
       <c r="AJ33">
-        <v>0.71151900000000001</v>
+        <v>0.75405199999999994</v>
       </c>
       <c r="AK33">
-        <v>0.75405199999999994</v>
+        <v>0.740116</v>
       </c>
       <c r="AL33">
-        <v>0.740116</v>
+        <v>0.72936199999999995</v>
       </c>
       <c r="AM33">
-        <v>0.72936199999999995</v>
+        <v>0.72201599999999999</v>
       </c>
       <c r="AN33">
-        <v>0.72201599999999999</v>
+        <v>0.75213099999999999</v>
       </c>
       <c r="AO33">
-        <v>0.75213099999999999</v>
+        <v>0.77636799999999995</v>
       </c>
       <c r="AP33">
-        <v>0.77636799999999995</v>
+        <v>0.88120100000000001</v>
       </c>
       <c r="AQ33">
-        <v>0.88120100000000001</v>
-      </c>
-      <c r="AR33">
         <v>0.86880000000000002</v>
       </c>
-      <c r="AS33">
-        <v>0.86193200000000003</v>
-      </c>
     </row>
-    <row r="34" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>6.9</v>
       </c>
@@ -6689,7 +6495,7 @@
         <v>0.74983100000000003</v>
       </c>
       <c r="AA34">
-        <v>0.76830200000000004</v>
+        <v>0.77684200000000003</v>
       </c>
       <c r="AB34">
         <v>0.78487300000000004</v>
@@ -6716,37 +6522,31 @@
         <v>0.661798</v>
       </c>
       <c r="AJ34">
-        <v>0.626884</v>
+        <v>0.66985099999999997</v>
       </c>
       <c r="AK34">
-        <v>0.66985099999999997</v>
+        <v>0.65610999999999997</v>
       </c>
       <c r="AL34">
-        <v>0.65610999999999997</v>
+        <v>0.64511499999999999</v>
       </c>
       <c r="AM34">
-        <v>0.64511499999999999</v>
+        <v>0.63743099999999997</v>
       </c>
       <c r="AN34">
-        <v>0.63743099999999997</v>
+        <v>0.66856099999999996</v>
       </c>
       <c r="AO34">
-        <v>0.66856099999999996</v>
+        <v>0.69287500000000002</v>
       </c>
       <c r="AP34">
-        <v>0.69287500000000002</v>
+        <v>0.79877399999999998</v>
       </c>
       <c r="AQ34">
-        <v>0.79877399999999998</v>
-      </c>
-      <c r="AR34">
         <v>0.78457200000000005</v>
       </c>
-      <c r="AS34">
-        <v>0.77684200000000003</v>
-      </c>
     </row>
-    <row r="35" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>8.4</v>
       </c>
@@ -6826,7 +6626,7 @@
         <v>0.67796900000000004</v>
       </c>
       <c r="AA35">
-        <v>0.69726699999999997</v>
+        <v>0.70629699999999995</v>
       </c>
       <c r="AB35">
         <v>0.71466700000000005</v>
@@ -6853,37 +6653,31 @@
         <v>0.59341200000000005</v>
       </c>
       <c r="AJ35">
-        <v>0.55843200000000004</v>
+        <v>0.60148900000000005</v>
       </c>
       <c r="AK35">
-        <v>0.60148900000000005</v>
+        <v>0.58814500000000003</v>
       </c>
       <c r="AL35">
-        <v>0.58814500000000003</v>
+        <v>0.57713700000000001</v>
       </c>
       <c r="AM35">
-        <v>0.57713700000000001</v>
+        <v>0.56933199999999995</v>
       </c>
       <c r="AN35">
-        <v>0.56933199999999995</v>
+        <v>0.60087800000000002</v>
       </c>
       <c r="AO35">
-        <v>0.60087800000000002</v>
+        <v>0.62481299999999995</v>
       </c>
       <c r="AP35">
-        <v>0.62481299999999995</v>
+        <v>0.72938099999999995</v>
       </c>
       <c r="AQ35">
-        <v>0.72938099999999995</v>
-      </c>
-      <c r="AR35">
         <v>0.71440400000000004</v>
       </c>
-      <c r="AS35">
-        <v>0.70629699999999995</v>
-      </c>
     </row>
-    <row r="36" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>9.8000000000000007</v>
       </c>
@@ -6963,7 +6757,7 @@
         <v>0.614209</v>
       </c>
       <c r="AA36">
-        <v>0.63363400000000003</v>
+        <v>0.64243499999999998</v>
       </c>
       <c r="AB36">
         <v>0.65127699999999999</v>
@@ -6990,37 +6784,31 @@
         <v>0.53293199999999996</v>
       </c>
       <c r="AJ36">
-        <v>0.49830799999999997</v>
+        <v>0.54078199999999998</v>
       </c>
       <c r="AK36">
-        <v>0.54078199999999998</v>
+        <v>0.52810100000000004</v>
       </c>
       <c r="AL36">
-        <v>0.52810100000000004</v>
+        <v>0.51728499999999999</v>
       </c>
       <c r="AM36">
-        <v>0.51728499999999999</v>
+        <v>0.50955600000000001</v>
       </c>
       <c r="AN36">
-        <v>0.50955600000000001</v>
+        <v>0.54129799999999995</v>
       </c>
       <c r="AO36">
-        <v>0.54129799999999995</v>
+        <v>0.56489699999999998</v>
       </c>
       <c r="AP36">
-        <v>0.56489699999999998</v>
+        <v>0.66593899999999995</v>
       </c>
       <c r="AQ36">
-        <v>0.66593899999999995</v>
-      </c>
-      <c r="AR36">
         <v>0.65066000000000002</v>
       </c>
-      <c r="AS36">
-        <v>0.64243499999999998</v>
-      </c>
     </row>
-    <row r="37" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>19.899989999999999</v>
       </c>
@@ -7100,7 +6888,7 @@
         <v>0.31273899999999999</v>
       </c>
       <c r="AA37">
-        <v>0.33026</v>
+        <v>0.33836500000000003</v>
       </c>
       <c r="AB37">
         <v>0.34600999999999998</v>
@@ -7127,37 +6915,31 @@
         <v>0.23730799999999999</v>
       </c>
       <c r="AJ37">
-        <v>0.20405599999999999</v>
+        <v>0.243257</v>
       </c>
       <c r="AK37">
-        <v>0.243257</v>
+        <v>0.236093</v>
       </c>
       <c r="AL37">
-        <v>0.236093</v>
+        <v>0.22773399999999999</v>
       </c>
       <c r="AM37">
-        <v>0.22773399999999999</v>
+        <v>0.22190399999999999</v>
       </c>
       <c r="AN37">
-        <v>0.22190399999999999</v>
+        <v>0.25459199999999998</v>
       </c>
       <c r="AO37">
-        <v>0.25459199999999998</v>
+        <v>0.27725100000000003</v>
       </c>
       <c r="AP37">
-        <v>0.27725100000000003</v>
+        <v>0.35950300000000002</v>
       </c>
       <c r="AQ37">
-        <v>0.35950300000000002</v>
-      </c>
-      <c r="AR37">
         <v>0.34565000000000001</v>
       </c>
-      <c r="AS37">
-        <v>0.33836500000000003</v>
-      </c>
     </row>
-    <row r="38" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>24.899989999999999</v>
       </c>
@@ -7237,7 +7019,7 @@
         <v>0.207035</v>
       </c>
       <c r="AA38">
-        <v>0.222771</v>
+        <v>0.230155</v>
       </c>
       <c r="AB38">
         <v>0.23685200000000001</v>
@@ -7264,37 +7046,31 @@
         <v>0.126856</v>
       </c>
       <c r="AJ38">
-        <v>9.3951999999999994E-2</v>
+        <v>0.13161800000000001</v>
       </c>
       <c r="AK38">
-        <v>0.13161800000000001</v>
+        <v>0.12734200000000001</v>
       </c>
       <c r="AL38">
-        <v>0.12734200000000001</v>
+        <v>0.120533</v>
       </c>
       <c r="AM38">
-        <v>0.120533</v>
+        <v>0.11602999999999999</v>
       </c>
       <c r="AN38">
-        <v>0.11602999999999999</v>
+        <v>0.149171</v>
       </c>
       <c r="AO38">
-        <v>0.149171</v>
+        <v>0.17200099999999999</v>
       </c>
       <c r="AP38">
-        <v>0.17200099999999999</v>
+        <v>0.24879799999999999</v>
       </c>
       <c r="AQ38">
-        <v>0.24879799999999999</v>
-      </c>
-      <c r="AR38">
         <v>0.236536</v>
       </c>
-      <c r="AS38">
-        <v>0.230155</v>
-      </c>
     </row>
-    <row r="39" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>29.899989999999999</v>
       </c>
@@ -7374,7 +7150,7 @@
         <v>0.12338300000000001</v>
       </c>
       <c r="AA39">
-        <v>0.137402</v>
+        <v>0.14385899999999999</v>
       </c>
       <c r="AB39">
         <v>0.14976200000000001</v>
@@ -7401,37 +7177,31 @@
         <v>3.5452999999999998E-2</v>
       </c>
       <c r="AJ39">
-        <v>2.539E-3</v>
+        <v>3.8974000000000002E-2</v>
       </c>
       <c r="AK39">
-        <v>3.8974000000000002E-2</v>
+        <v>3.7421999999999997E-2</v>
       </c>
       <c r="AL39">
-        <v>3.7421999999999997E-2</v>
+        <v>3.2086999999999997E-2</v>
       </c>
       <c r="AM39">
-        <v>3.2086999999999997E-2</v>
+        <v>2.9017000000000001E-2</v>
       </c>
       <c r="AN39">
-        <v>2.9017000000000001E-2</v>
+        <v>6.2939999999999996E-2</v>
       </c>
       <c r="AO39">
-        <v>6.2939999999999996E-2</v>
+        <v>8.6983000000000005E-2</v>
       </c>
       <c r="AP39">
-        <v>8.6983000000000005E-2</v>
+        <v>0.16012899999999999</v>
       </c>
       <c r="AQ39">
-        <v>0.16012899999999999</v>
-      </c>
-      <c r="AR39">
         <v>0.149446</v>
       </c>
-      <c r="AS39">
-        <v>0.14385899999999999</v>
-      </c>
     </row>
-    <row r="40" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>34.9</v>
       </c>
@@ -7511,7 +7281,7 @@
         <v>4.6474000000000001E-2</v>
       </c>
       <c r="AA40">
-        <v>5.8694999999999997E-2</v>
+        <v>6.4101000000000005E-2</v>
       </c>
       <c r="AB40">
         <v>6.9100999999999996E-2</v>
@@ -7538,37 +7308,31 @@
         <v>-5.2025000000000002E-2</v>
       </c>
       <c r="AJ40">
-        <v>-8.6243E-2</v>
+        <v>-4.9772999999999998E-2</v>
       </c>
       <c r="AK40">
-        <v>-4.9772999999999998E-2</v>
+        <v>-4.8457E-2</v>
       </c>
       <c r="AL40">
-        <v>-4.8457E-2</v>
+        <v>-5.2328E-2</v>
       </c>
       <c r="AM40">
-        <v>-5.2328E-2</v>
+        <v>-5.3740000000000003E-2</v>
       </c>
       <c r="AN40">
-        <v>-5.3740000000000003E-2</v>
+        <v>-1.7693E-2</v>
       </c>
       <c r="AO40">
-        <v>-1.7693E-2</v>
+        <v>7.045E-3</v>
       </c>
       <c r="AP40">
-        <v>7.045E-3</v>
+        <v>7.7661999999999995E-2</v>
       </c>
       <c r="AQ40">
-        <v>7.7661999999999995E-2</v>
-      </c>
-      <c r="AR40">
         <v>6.8683999999999995E-2</v>
       </c>
-      <c r="AS40">
-        <v>6.4101000000000005E-2</v>
-      </c>
     </row>
-    <row r="41" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -7648,7 +7412,7 @@
         <v>-1.9186000000000002E-2</v>
       </c>
       <c r="AA41">
-        <v>-9.0069999999999994E-3</v>
+        <v>-4.4869999999999997E-3</v>
       </c>
       <c r="AB41">
         <v>-6.0599999999999998E-4</v>
@@ -7675,37 +7439,31 @@
         <v>-0.13084000000000001</v>
       </c>
       <c r="AJ41">
-        <v>-0.165909</v>
+        <v>-0.12998399999999999</v>
       </c>
       <c r="AK41">
-        <v>-0.12998399999999999</v>
+        <v>-0.125696</v>
       </c>
       <c r="AL41">
-        <v>-0.125696</v>
+        <v>-0.12786500000000001</v>
       </c>
       <c r="AM41">
-        <v>-0.12786500000000001</v>
+        <v>-0.12750400000000001</v>
       </c>
       <c r="AN41">
-        <v>-0.12750400000000001</v>
+        <v>-8.9835999999999999E-2</v>
       </c>
       <c r="AO41">
-        <v>-8.9835999999999999E-2</v>
+        <v>-6.3464999999999994E-2</v>
       </c>
       <c r="AP41">
-        <v>-6.3464999999999994E-2</v>
+        <v>6.038E-3</v>
       </c>
       <c r="AQ41">
-        <v>6.038E-3</v>
-      </c>
-      <c r="AR41">
         <v>-9.3099999999999997E-4</v>
       </c>
-      <c r="AS41">
-        <v>-4.4869999999999997E-3</v>
-      </c>
     </row>
-    <row r="42" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>45</v>
       </c>
@@ -7785,7 +7543,7 @@
         <v>-4.8549000000000002E-2</v>
       </c>
       <c r="AA42">
-        <v>-4.0633000000000002E-2</v>
+        <v>-3.7187999999999999E-2</v>
       </c>
       <c r="AB42">
         <v>-3.4521000000000003E-2</v>
@@ -7812,37 +7570,31 @@
         <v>-0.171685</v>
       </c>
       <c r="AJ42">
-        <v>-0.20696000000000001</v>
+        <v>-0.172232</v>
       </c>
       <c r="AK42">
-        <v>-0.172232</v>
+        <v>-0.16525899999999999</v>
       </c>
       <c r="AL42">
-        <v>-0.16525899999999999</v>
+        <v>-0.165829</v>
       </c>
       <c r="AM42">
-        <v>-0.165829</v>
+        <v>-0.163628</v>
       </c>
       <c r="AN42">
-        <v>-0.163628</v>
+        <v>-0.12463100000000001</v>
       </c>
       <c r="AO42">
-        <v>-0.12463100000000001</v>
+        <v>-9.7185999999999995E-2</v>
       </c>
       <c r="AP42">
-        <v>-9.7185999999999995E-2</v>
+        <v>-2.9899999999999999E-2</v>
       </c>
       <c r="AQ42">
-        <v>-2.9899999999999999E-2</v>
-      </c>
-      <c r="AR42">
         <v>-3.4763000000000002E-2</v>
       </c>
-      <c r="AS42">
-        <v>-3.7187999999999999E-2</v>
-      </c>
     </row>
-    <row r="43" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>49.599989999999998</v>
       </c>
@@ -7922,7 +7674,7 @@
         <v>-5.9847999999999998E-2</v>
       </c>
       <c r="AA43">
-        <v>-5.4260999999999997E-2</v>
+        <v>-5.1905E-2</v>
       </c>
       <c r="AB43">
         <v>-5.0428000000000001E-2</v>
@@ -7949,37 +7701,31 @@
         <v>-0.19430700000000001</v>
       </c>
       <c r="AJ43">
-        <v>-0.229627</v>
+        <v>-0.19620799999999999</v>
       </c>
       <c r="AK43">
-        <v>-0.19620799999999999</v>
+        <v>-0.18676699999999999</v>
       </c>
       <c r="AL43">
-        <v>-0.18676699999999999</v>
+        <v>-0.185752</v>
       </c>
       <c r="AM43">
-        <v>-0.185752</v>
+        <v>-0.181756</v>
       </c>
       <c r="AN43">
-        <v>-0.181756</v>
+        <v>-0.14177300000000001</v>
       </c>
       <c r="AO43">
-        <v>-0.14177300000000001</v>
+        <v>-0.113136</v>
       </c>
       <c r="AP43">
-        <v>-0.113136</v>
+        <v>-4.7941999999999999E-2</v>
       </c>
       <c r="AQ43">
-        <v>-4.7941999999999999E-2</v>
-      </c>
-      <c r="AR43">
         <v>-5.0687000000000003E-2</v>
       </c>
-      <c r="AS43">
-        <v>-5.1905E-2</v>
-      </c>
     </row>
-    <row r="44" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>55.099989999999998</v>
       </c>
@@ -8059,7 +7805,7 @@
         <v>-6.0610999999999998E-2</v>
       </c>
       <c r="AA44">
-        <v>-5.7231999999999998E-2</v>
+        <v>-5.5975999999999998E-2</v>
       </c>
       <c r="AB44">
         <v>-5.5638E-2</v>
@@ -8086,37 +7832,31 @@
         <v>-0.20627400000000001</v>
       </c>
       <c r="AJ44">
-        <v>-0.241563</v>
+        <v>-0.209479</v>
       </c>
       <c r="AK44">
-        <v>-0.209479</v>
+        <v>-0.197764</v>
       </c>
       <c r="AL44">
-        <v>-0.197764</v>
+        <v>-0.19526099999999999</v>
       </c>
       <c r="AM44">
-        <v>-0.19526099999999999</v>
+        <v>-0.189498</v>
       </c>
       <c r="AN44">
-        <v>-0.189498</v>
+        <v>-0.148149</v>
       </c>
       <c r="AO44">
-        <v>-0.148149</v>
+        <v>-0.118295</v>
       </c>
       <c r="AP44">
-        <v>-0.118295</v>
+        <v>-5.5248999999999999E-2</v>
       </c>
       <c r="AQ44">
-        <v>-5.5248999999999999E-2</v>
-      </c>
-      <c r="AR44">
         <v>-5.5858999999999999E-2</v>
       </c>
-      <c r="AS44">
-        <v>-5.5975999999999998E-2</v>
-      </c>
     </row>
-    <row r="45" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>60.099989999999998</v>
       </c>
@@ -8196,7 +7936,7 @@
         <v>-5.9527999999999998E-2</v>
       </c>
       <c r="AA45">
-        <v>-5.8546000000000001E-2</v>
+        <v>-5.8434E-2</v>
       </c>
       <c r="AB45">
         <v>-5.9455000000000001E-2</v>
@@ -8223,37 +7963,31 @@
         <v>-0.21910199999999999</v>
       </c>
       <c r="AJ45">
-        <v>-0.25435000000000002</v>
+        <v>-0.22367400000000001</v>
       </c>
       <c r="AK45">
-        <v>-0.22367400000000001</v>
+        <v>-0.209535</v>
       </c>
       <c r="AL45">
-        <v>-0.209535</v>
+        <v>-0.205425</v>
       </c>
       <c r="AM45">
-        <v>-0.205425</v>
+        <v>-0.19764499999999999</v>
       </c>
       <c r="AN45">
-        <v>-0.19764499999999999</v>
+        <v>-0.15409700000000001</v>
       </c>
       <c r="AO45">
-        <v>-0.15409700000000001</v>
+        <v>-0.122727</v>
       </c>
       <c r="AP45">
-        <v>-0.122727</v>
+        <v>-6.1315000000000001E-2</v>
       </c>
       <c r="AQ45">
-        <v>-6.1315000000000001E-2</v>
-      </c>
-      <c r="AR45">
         <v>-5.9612999999999999E-2</v>
       </c>
-      <c r="AS45">
-        <v>-5.8434E-2</v>
-      </c>
     </row>
-    <row r="46" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>69.900000000000006</v>
       </c>
@@ -8333,7 +8067,7 @@
         <v>-3.5346000000000002E-2</v>
       </c>
       <c r="AA46">
-        <v>-3.8801000000000002E-2</v>
+        <v>-4.0846E-2</v>
       </c>
       <c r="AB46">
         <v>-4.4247000000000002E-2</v>
@@ -8360,37 +8094,31 @@
         <v>-0.22159300000000001</v>
       </c>
       <c r="AJ46">
-        <v>-0.25571100000000002</v>
+        <v>-0.22855600000000001</v>
       </c>
       <c r="AK46">
-        <v>-0.22855600000000001</v>
+        <v>-0.21055099999999999</v>
       </c>
       <c r="AL46">
-        <v>-0.21055099999999999</v>
+        <v>-0.203679</v>
       </c>
       <c r="AM46">
-        <v>-0.203679</v>
+        <v>-0.19228899999999999</v>
       </c>
       <c r="AN46">
-        <v>-0.19228899999999999</v>
+        <v>-0.14480699999999999</v>
       </c>
       <c r="AO46">
-        <v>-0.14480699999999999</v>
+        <v>-0.109746</v>
       </c>
       <c r="AP46">
-        <v>-0.109746</v>
+        <v>-5.0248000000000001E-2</v>
       </c>
       <c r="AQ46">
-        <v>-5.0248000000000001E-2</v>
-      </c>
-      <c r="AR46">
         <v>-4.4394000000000003E-2</v>
       </c>
-      <c r="AS46">
-        <v>-4.0846E-2</v>
-      </c>
     </row>
-    <row r="47" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>75</v>
       </c>
@@ -8470,7 +8198,7 @@
         <v>-2.2804000000000001E-2</v>
       </c>
       <c r="AA47">
-        <v>-2.8672E-2</v>
+        <v>-3.1980000000000001E-2</v>
       </c>
       <c r="AB47">
         <v>-3.6728999999999998E-2</v>
@@ -8497,37 +8225,31 @@
         <v>-0.22550799999999999</v>
       </c>
       <c r="AJ47">
-        <v>-0.25877299999999998</v>
+        <v>-0.233686</v>
       </c>
       <c r="AK47">
-        <v>-0.233686</v>
+        <v>-0.21375</v>
       </c>
       <c r="AL47">
-        <v>-0.21375</v>
+        <v>-0.20539099999999999</v>
       </c>
       <c r="AM47">
-        <v>-0.20539099999999999</v>
+        <v>-0.191832</v>
       </c>
       <c r="AN47">
-        <v>-0.191832</v>
+        <v>-0.14114499999999999</v>
       </c>
       <c r="AO47">
-        <v>-0.14114499999999999</v>
+        <v>-0.103966</v>
       </c>
       <c r="AP47">
-        <v>-0.103966</v>
+        <v>-4.5060000000000003E-2</v>
       </c>
       <c r="AQ47">
-        <v>-4.5060000000000003E-2</v>
-      </c>
-      <c r="AR47">
         <v>-3.6868999999999999E-2</v>
       </c>
-      <c r="AS47">
-        <v>-3.1980000000000001E-2</v>
-      </c>
     </row>
-    <row r="48" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>80</v>
       </c>
@@ -8607,7 +8329,7 @@
         <v>-1.8168E-2</v>
       </c>
       <c r="AA48">
-        <v>-2.7348000000000001E-2</v>
+        <v>-3.2125000000000001E-2</v>
       </c>
       <c r="AB48">
         <v>-3.8656000000000003E-2</v>
@@ -8634,37 +8356,31 @@
         <v>-0.245309</v>
       </c>
       <c r="AJ48">
-        <v>-0.276642</v>
+        <v>-0.25494800000000001</v>
       </c>
       <c r="AK48">
-        <v>-0.25494800000000001</v>
+        <v>-0.232709</v>
       </c>
       <c r="AL48">
-        <v>-0.232709</v>
+        <v>-0.22244</v>
       </c>
       <c r="AM48">
-        <v>-0.22244</v>
+        <v>-0.20613899999999999</v>
       </c>
       <c r="AN48">
-        <v>-0.20613899999999999</v>
+        <v>-0.15019299999999999</v>
       </c>
       <c r="AO48">
-        <v>-0.15019299999999999</v>
+        <v>-0.108877</v>
       </c>
       <c r="AP48">
-        <v>-0.108877</v>
+        <v>-5.0019000000000001E-2</v>
       </c>
       <c r="AQ48">
-        <v>-5.0019000000000001E-2</v>
-      </c>
-      <c r="AR48">
         <v>-3.8795000000000003E-2</v>
       </c>
-      <c r="AS48">
-        <v>-3.2125000000000001E-2</v>
-      </c>
     </row>
-    <row r="49" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>90</v>
       </c>
@@ -8744,7 +8460,7 @@
         <v>-2.5912999999999999E-2</v>
       </c>
       <c r="AA49">
-        <v>-4.2783000000000002E-2</v>
+        <v>-5.1293999999999999E-2</v>
       </c>
       <c r="AB49">
         <v>-6.2696000000000002E-2</v>
@@ -8771,37 +8487,31 @@
         <v>-0.301375</v>
       </c>
       <c r="AJ49">
-        <v>-0.34095999999999999</v>
+        <v>-0.316581</v>
       </c>
       <c r="AK49">
-        <v>-0.316581</v>
+        <v>-0.28458099999999997</v>
       </c>
       <c r="AL49">
-        <v>-0.28458099999999997</v>
+        <v>-0.27049200000000001</v>
       </c>
       <c r="AM49">
-        <v>-0.27049200000000001</v>
+        <v>-0.247445</v>
       </c>
       <c r="AN49">
-        <v>-0.247445</v>
+        <v>-0.19966500000000001</v>
       </c>
       <c r="AO49">
-        <v>-0.19966500000000001</v>
+        <v>-0.148592</v>
       </c>
       <c r="AP49">
-        <v>-0.148592</v>
+        <v>-8.2361000000000004E-2</v>
       </c>
       <c r="AQ49">
-        <v>-8.2361000000000004E-2</v>
-      </c>
-      <c r="AR49">
         <v>-6.2898999999999997E-2</v>
       </c>
-      <c r="AS49">
-        <v>-5.1293999999999999E-2</v>
-      </c>
     </row>
-    <row r="50" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>100</v>
       </c>
@@ -8881,7 +8591,7 @@
         <v>-0.13428100000000001</v>
       </c>
       <c r="AA50">
-        <v>-0.186776</v>
+        <v>-0.20932400000000001</v>
       </c>
       <c r="AB50">
         <v>-0.23294200000000001</v>
@@ -8908,34 +8618,28 @@
         <v>-0.62547200000000003</v>
       </c>
       <c r="AJ50">
-        <v>-0.60192400000000001</v>
+        <v>-0.648594</v>
       </c>
       <c r="AK50">
-        <v>-0.648594</v>
+        <v>-0.62358100000000005</v>
       </c>
       <c r="AL50">
-        <v>-0.62358100000000005</v>
+        <v>-0.59192599999999995</v>
       </c>
       <c r="AM50">
-        <v>-0.59192599999999995</v>
+        <v>-0.53808800000000001</v>
       </c>
       <c r="AN50">
-        <v>-0.53808800000000001</v>
+        <v>-0.36381000000000002</v>
       </c>
       <c r="AO50">
-        <v>-0.36381000000000002</v>
+        <v>-0.30522899999999997</v>
       </c>
       <c r="AP50">
-        <v>-0.30522899999999997</v>
+        <v>-0.26976899999999998</v>
       </c>
       <c r="AQ50">
-        <v>-0.26976899999999998</v>
-      </c>
-      <c r="AR50">
         <v>-0.23375000000000001</v>
-      </c>
-      <c r="AS50">
-        <v>-0.20932400000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>